<commit_message>
Catalogo de productos 1.0
</commit_message>
<xml_diff>
--- a/reportes/base/ocatalogoProductos.xlsx
+++ b/reportes/base/ocatalogoProductos.xlsx
@@ -5,22 +5,34 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4003299a955809c3/Escritorio/calera/reportes/base/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uemar\Desktop\calera\report_sa_services\reportes\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="11_A3AD8052060DDFB58B4CFB36282AC21238724DF3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49931386-E980-4E6D-9D19-281DB7013256}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88F0FB1-726B-4543-BAA6-A2644F7453B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="21580" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Catálogo de productos</t>
   </si>
@@ -31,14 +43,17 @@
     <t>Descripcion</t>
   </si>
   <si>
-    <t xml:space="preserve">Nombre corto	</t>
+    <t>Fecha:</t>
+  </si>
+  <si>
+    <t>Nombre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +95,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aparajita"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -116,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -130,6 +151,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -446,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -466,29 +494,34 @@
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" ht="6.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="4" t="s">
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="9">
+        <f ca="1">TODAY()</f>
+        <v>44780</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="6.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>3</v>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -504,7 +537,7 @@
     <row r="8" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
@@ -660,6 +693,11 @@
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Catalogo de productos FINALIZADO
</commit_message>
<xml_diff>
--- a/reportes/base/ocatalogoProductos.xlsx
+++ b/reportes/base/ocatalogoProductos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uemar\Desktop\calera\report_sa_services\reportes\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88F0FB1-726B-4543-BAA6-A2644F7453B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DA5C27-BE8C-4B0F-AFBB-F77895483FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="10" windowWidth="21580" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,14 +150,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -477,7 +477,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -488,18 +488,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <f ca="1">TODAY()</f>
         <v>44780</v>
       </c>
@@ -521,7 +521,7 @@
     </row>
     <row r="5" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
-      <c r="B5" s="5"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Catalogo de productos FINALIZADO con existencia en almacen
</commit_message>
<xml_diff>
--- a/reportes/base/ocatalogoProductos.xlsx
+++ b/reportes/base/ocatalogoProductos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uemar\Desktop\calera\report_sa_services\reportes\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DA5C27-BE8C-4B0F-AFBB-F77895483FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA39139-F105-4737-9EE2-E1CE700070BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="10" windowWidth="21580" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Catálogo de productos</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Nombre</t>
+  </si>
+  <si>
+    <t>Existencia Almacen</t>
   </si>
 </sst>
 </file>
@@ -474,41 +477,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.54296875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="58" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.36328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="53.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
-    </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D1"/>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6"/>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8">
+      <c r="D2" s="8">
         <f ca="1">TODAY()</f>
         <v>44780</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="6.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="6.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -518,186 +523,225 @@
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
-    </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
-    </row>
-    <row r="37" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
-    </row>
-    <row r="40" spans="1:3" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Reporte de Estadistica de clientes
</commit_message>
<xml_diff>
--- a/reportes/base/ocatalogoProductos.xlsx
+++ b/reportes/base/ocatalogoProductos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uemar\Desktop\calera\report_sa_services\reportes\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA39139-F105-4737-9EE2-E1CE700070BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1E1BC1-0529-4101-8342-EFB12677942E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="10" windowWidth="21580" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,13 +90,6 @@
       <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Aparajita"/>
       <family val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -140,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -150,14 +143,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -480,7 +470,7 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -492,19 +482,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
       <c r="D1"/>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="6"/>
-      <c r="C2" s="7" t="s">
+      <c r="A2" s="5"/>
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <f ca="1">TODAY()</f>
         <v>44780</v>
       </c>
@@ -543,13 +533,13 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="5"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>

</xml_diff>